<commit_message>
University Program view, add, update, import, export, bulk update
</commit_message>
<xml_diff>
--- a/public/format/university-program-list.xlsx
+++ b/public/format/university-program-list.xlsx
@@ -14,10 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>program_name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>course_category_id</t>
   </si>
@@ -25,24 +22,12 @@
     <t>specialization_id</t>
   </si>
   <si>
-    <t>level_id</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
     <t>study_mode</t>
   </si>
   <si>
-    <t>tution_fees</t>
-  </si>
-  <si>
-    <t>course_mode</t>
-  </si>
-  <si>
-    <t>exam_accepted</t>
-  </si>
-  <si>
     <t>intake</t>
   </si>
   <si>
@@ -52,25 +37,25 @@
     <t>entry_requirement</t>
   </si>
   <si>
-    <t>ielts</t>
-  </si>
-  <si>
-    <t>toefl</t>
-  </si>
-  <si>
-    <t>pte</t>
-  </si>
-  <si>
-    <t>duolingo</t>
-  </si>
-  <si>
-    <t>gre</t>
-  </si>
-  <si>
-    <t>gmat</t>
-  </si>
-  <si>
-    <t>sat</t>
+    <t>course_name</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>application_deadline</t>
+  </si>
+  <si>
+    <t>tution_fee</t>
+  </si>
+  <si>
+    <t>exam_required</t>
+  </si>
+  <si>
+    <t>mode_of_instruction</t>
+  </si>
+  <si>
+    <t>scholarship_info</t>
   </si>
 </sst>
 </file>
@@ -899,47 +884,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="8" max="8" width="27.26953125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
       </c>
       <c r="L1" t="s">
         <v>11</v>
@@ -949,21 +937,6 @@
       </c>
       <c r="N1" t="s">
         <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>